<commit_message>
generate new vocab exports
</commit_message>
<xml_diff>
--- a/storage/app/public/vocabs/testbeds/1.3/testbeds_1-3.xlsx
+++ b/storage/app/public/vocabs/testbeds/1.3/testbeds_1-3.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="248">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="249">
   <si>
     <t>synonyms</t>
   </si>
@@ -206,19 +206,19 @@
     <t>https://epos-msl.uu.nl/voc/testbeds/1.3/facility_types</t>
   </si>
   <si>
-    <t>geoenergy testbed</t>
-  </si>
-  <si>
-    <t>#geo-energy testbed#geoenergy test bed#geo-energy test bed#krafla#magma testbed#magma test bed</t>
-  </si>
-  <si>
-    <t>https://epos-msl.uu.nl/voc/testbeds/1.3/facility_types-geoenergy_testbed</t>
+    <t>geo-energy testbed</t>
+  </si>
+  <si>
+    <t>#geoenergy testbed#geoenergy test bed#geo-energy test bed#krafla#magma testbed#magma test bed</t>
+  </si>
+  <si>
+    <t>https://epos-msl.uu.nl/voc/testbeds/1.3/facility_types-geo-energy_testbed</t>
   </si>
   <si>
     <t>in-situ laboratory</t>
   </si>
   <si>
-    <t>#in-situ lab#underground laboratory#subsurface laboratory#subsurface infrastructure#bedrottolab</t>
+    <t>#in-situ lab#underground laboratory#subsurface laboratory#subsurface infrastructure#bedrottolab#insitu lab#in situ lab#nsitu laboratory#in situ laboratory</t>
   </si>
   <si>
     <t>https://epos-msl.uu.nl/voc/testbeds/1.3/facility_types-in-situ_laboratory</t>
@@ -227,6 +227,9 @@
     <t>field-scale laboratory - active testing</t>
   </si>
   <si>
+    <t>#full-scale testing laboratory#full scale testing laboratory#testing at full-scale</t>
+  </si>
+  <si>
     <t>https://epos-msl.uu.nl/voc/testbeds/1.3/facility_types-field-scale_laboratory_-_active_testing</t>
   </si>
   <si>
@@ -239,19 +242,10 @@
     <t>https://epos-msl.uu.nl/voc/testbeds/1.3/facility_types-field-scale_observatory_-_passive_monitoring</t>
   </si>
   <si>
-    <t>full-scale testing laboratory</t>
-  </si>
-  <si>
-    <t>#full scale testing laboratory#testing at full-scale</t>
-  </si>
-  <si>
-    <t>https://epos-msl.uu.nl/voc/testbeds/1.3/facility_types-full-scale_testing_laboratory</t>
-  </si>
-  <si>
     <t>monitoring borehole</t>
   </si>
   <si>
-    <t>#monitoring wellbore</t>
+    <t>#monitoring wellbore#monitoring well</t>
   </si>
   <si>
     <t>https://epos-msl.uu.nl/voc/testbeds/1.3/facility_types-monitoring_borehole</t>
@@ -275,7 +269,7 @@
     <t>three-component seismic station</t>
   </si>
   <si>
-    <t>#seismic borehole#seismic monitoring borehole</t>
+    <t>#seismic borehole#seismic monitoring borehole#three-component seismometer#three component seismometer</t>
   </si>
   <si>
     <t>https://epos-msl.uu.nl/voc/testbeds/1.3/equipment-seismic_monitoring-three-component_seismic_station</t>
@@ -284,7 +278,7 @@
     <t>tilt strain gauge</t>
   </si>
   <si>
-    <t>#tilt gauge#tiltmeter#tilt meter</t>
+    <t>#tilt gauge#tiltmeter#tilt meter#tilt-strain gauge</t>
   </si>
   <si>
     <t>https://epos-msl.uu.nl/voc/testbeds/1.3/equipment-seismic_monitoring-tilt_strain_gauge</t>
@@ -347,24 +341,36 @@
     <t>borehole geophone</t>
   </si>
   <si>
+    <t>#downhole geophone#borehole triaxial geophone</t>
+  </si>
+  <si>
     <t>https://epos-msl.uu.nl/voc/testbeds/1.3/equipment-borehole_monitoring-borehole_geophone</t>
   </si>
   <si>
     <t>downhole electromagnetic sensing</t>
   </si>
   <si>
+    <t>#downhole electromagnetic sensors#borehole electromagnetic sensing#borehole electromagnetic sensor#downhole em sensing#downhole em sensors#borehole em sensing#borehole em sensor#downhole magnetoelastic sensing#borehole magnetoelastic sensing#downhole magnetoelastic sensor#borehole magnetoelastic sensor</t>
+  </si>
+  <si>
     <t>https://epos-msl.uu.nl/voc/testbeds/1.3/equipment-borehole_monitoring-downhole_electromagnetic_sensing</t>
   </si>
   <si>
     <t>downhole electric conductivity sensing</t>
   </si>
   <si>
+    <t>#downhole electric conductivity sensor#borehole electric conductivity sensing#borehole electric conductivity sensor#downhole specific conductance sensing#downhole specific conductance sensor#borehole specific conductance sensing#borehole specific conductance sensor#downhole ec sensing#downhole ec sensor#borehole ec sensing#borehole ec sensor</t>
+  </si>
+  <si>
     <t>https://epos-msl.uu.nl/voc/testbeds/1.3/equipment-borehole_monitoring-downhole_electric_conductivity_sensing</t>
   </si>
   <si>
     <t>downhole soil gas probe</t>
   </si>
   <si>
+    <t>#downhole soil gas monitoring#downhole soil gas sensor#borehole soil gas probe#borehole soil gas monitoring#borehole soil gas sensor</t>
+  </si>
+  <si>
     <t>https://epos-msl.uu.nl/voc/testbeds/1.3/equipment-borehole_monitoring-downhole_soil_gas_probe</t>
   </si>
   <si>
@@ -401,7 +407,7 @@
     <t>intervention and stimulation equipment</t>
   </si>
   <si>
-    <t>#(ise)</t>
+    <t>#(ise)#intervention and stimulation solutions#intervention and stimulation solution#well intervention#well stimulation#borehole ntervention#borehole stimulation#wellbore ntervention#wellbore stimulation</t>
   </si>
   <si>
     <t>https://epos-msl.uu.nl/voc/testbeds/1.3/equipment-borehole_testing-intervention_and_stimulation_equipment</t>
@@ -410,7 +416,7 @@
     <t>pressure performance system</t>
   </si>
   <si>
-    <t>#(pps)</t>
+    <t>#(pps)#pressure transient testing#pressure performance</t>
   </si>
   <si>
     <t>https://epos-msl.uu.nl/voc/testbeds/1.3/equipment-borehole_testing-pressure_performance_system</t>
@@ -458,28 +464,37 @@
     <t>mud logging</t>
   </si>
   <si>
+    <t>#mud logger#mud log#mudlog#mudlogging</t>
+  </si>
+  <si>
     <t>https://epos-msl.uu.nl/voc/testbeds/1.3/equipment-borehole_drilling-mud_logging</t>
   </si>
   <si>
     <t>drilling test rig</t>
   </si>
   <si>
+    <t>#drill test rig#drill testrig#drilling testrig</t>
+  </si>
+  <si>
     <t>https://epos-msl.uu.nl/voc/testbeds/1.3/equipment-borehole_drilling-drilling_test_rig</t>
   </si>
   <si>
     <t>borehole and geofluid simulator</t>
   </si>
   <si>
+    <t>#borehole simulator#geofluid simulator</t>
+  </si>
+  <si>
     <t>https://epos-msl.uu.nl/voc/testbeds/1.3/equipment-borehole_drilling-borehole_and_geofluid_simulator</t>
   </si>
   <si>
-    <t>rock samples</t>
-  </si>
-  <si>
-    <t>#drill core#core#drilling cuttings#reservoir water</t>
-  </si>
-  <si>
-    <t>https://epos-msl.uu.nl/voc/testbeds/1.3/equipment-borehole_drilling-rock_samples</t>
+    <t>drill core</t>
+  </si>
+  <si>
+    <t>#drilling cuttings#core scanning#cutting samples#drillcore#core samples#downhole coring#wellbore coring#well coring</t>
+  </si>
+  <si>
+    <t>https://epos-msl.uu.nl/voc/testbeds/1.3/equipment-borehole_drilling-drill_core</t>
   </si>
   <si>
     <t>borehole logging</t>
@@ -491,25 +506,13 @@
     <t>https://epos-msl.uu.nl/voc/testbeds/1.3/equipment-borehole_logging</t>
   </si>
   <si>
-    <t>open-hole logging</t>
-  </si>
-  <si>
-    <t>#cased-hole logging#cased hole logging#sidewall coring</t>
-  </si>
-  <si>
-    <t>https://epos-msl.uu.nl/voc/testbeds/1.3/equipment-borehole_logging-open-hole_logging</t>
-  </si>
-  <si>
-    <t>geothermal heating and cooling</t>
-  </si>
-  <si>
-    <t>https://epos-msl.uu.nl/voc/testbeds/1.3/equipment-geothermal_heating_and_cooling</t>
-  </si>
-  <si>
-    <t>https://epos-msl.uu.nl/voc/testbeds/1.3/equipment-geothermal_heating_and_cooling-heat_pump_test_rig</t>
-  </si>
-  <si>
-    <t>https://epos-msl.uu.nl/voc/testbeds/1.3/equipment-geothermal_heating_and_cooling-heat_pump_mobile_unit</t>
+    <t>open hole logging</t>
+  </si>
+  <si>
+    <t>#cased-hole logging#cased hole logging#sidewall coring#open-hole logging</t>
+  </si>
+  <si>
+    <t>https://epos-msl.uu.nl/voc/testbeds/1.3/equipment-borehole_logging-open_hole_logging</t>
   </si>
   <si>
     <t>Models</t>
@@ -1098,7 +1101,7 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:G91"/>
+  <dimension ref="A1:G87"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
       <selection activeCell="A1" sqref="A1"/>
@@ -1374,37 +1377,37 @@
       <c r="B25" t="s">
         <v>69</v>
       </c>
+      <c r="D25" t="s">
+        <v>70</v>
+      </c>
       <c r="E25" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="26" spans="1:7">
       <c r="B26" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D26" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E26" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="27" spans="1:7">
       <c r="B27" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D27" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E27" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="28" spans="1:7">
-      <c r="B28" t="s">
-        <v>77</v>
-      </c>
-      <c r="D28" t="s">
+      <c r="A28" t="s">
         <v>78</v>
       </c>
       <c r="E28" t="s">
@@ -1412,639 +1415,628 @@
       </c>
     </row>
     <row r="29" spans="1:7">
-      <c r="A29" t="s">
+      <c r="B29" t="s">
         <v>80</v>
       </c>
+      <c r="D29" t="s">
+        <v>81</v>
+      </c>
       <c r="E29" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="30" spans="1:7">
-      <c r="B30" t="s">
-        <v>82</v>
+      <c r="C30" t="s">
+        <v>83</v>
       </c>
       <c r="D30" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="E30" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="31" spans="1:7">
       <c r="C31" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D31" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="E31" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="32" spans="1:7">
-      <c r="C32" t="s">
-        <v>88</v>
+      <c r="B32" t="s">
+        <v>89</v>
       </c>
       <c r="D32" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="E32" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="33" spans="1:7">
-      <c r="B33" t="s">
-        <v>91</v>
+      <c r="C33" t="s">
+        <v>92</v>
       </c>
       <c r="D33" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="E33" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="34" spans="1:7">
       <c r="C34" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D34" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E34" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="35" spans="1:7">
       <c r="C35" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D35" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="E35" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="36" spans="1:7">
       <c r="C36" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D36" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="E36" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
     </row>
     <row r="37" spans="1:7">
-      <c r="C37" t="s">
-        <v>103</v>
+      <c r="B37" t="s">
+        <v>104</v>
       </c>
       <c r="D37" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="E37" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="38" spans="1:7">
-      <c r="B38" t="s">
-        <v>106</v>
+      <c r="C38" t="s">
+        <v>107</v>
       </c>
       <c r="D38" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="E38" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="39" spans="1:7">
       <c r="C39" t="s">
-        <v>109</v>
+        <v>110</v>
+      </c>
+      <c r="D39" t="s">
+        <v>111</v>
       </c>
       <c r="E39" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="40" spans="1:7">
       <c r="C40" t="s">
-        <v>111</v>
+        <v>113</v>
+      </c>
+      <c r="D40" t="s">
+        <v>114</v>
       </c>
       <c r="E40" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
     </row>
     <row r="41" spans="1:7">
       <c r="C41" t="s">
-        <v>113</v>
+        <v>116</v>
+      </c>
+      <c r="D41" t="s">
+        <v>117</v>
       </c>
       <c r="E41" t="s">
-        <v>114</v>
+        <v>118</v>
       </c>
     </row>
     <row r="42" spans="1:7">
-      <c r="C42" t="s">
-        <v>115</v>
+      <c r="B42" t="s">
+        <v>119</v>
+      </c>
+      <c r="D42" t="s">
+        <v>120</v>
       </c>
       <c r="E42" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
     </row>
     <row r="43" spans="1:7">
-      <c r="B43" t="s">
-        <v>117</v>
+      <c r="C43" t="s">
+        <v>122</v>
       </c>
       <c r="D43" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="E43" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
     </row>
     <row r="44" spans="1:7">
       <c r="C44" t="s">
-        <v>120</v>
-      </c>
-      <c r="D44" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="E44" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
     </row>
     <row r="45" spans="1:7">
       <c r="C45" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="E45" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
     </row>
     <row r="46" spans="1:7">
       <c r="C46" t="s">
-        <v>125</v>
+        <v>129</v>
+      </c>
+      <c r="D46" t="s">
+        <v>130</v>
       </c>
       <c r="E46" t="s">
-        <v>126</v>
+        <v>131</v>
       </c>
     </row>
     <row r="47" spans="1:7">
       <c r="C47" t="s">
-        <v>127</v>
+        <v>132</v>
       </c>
       <c r="D47" t="s">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="E47" t="s">
-        <v>129</v>
+        <v>134</v>
       </c>
     </row>
     <row r="48" spans="1:7">
       <c r="C48" t="s">
-        <v>130</v>
-      </c>
-      <c r="D48" t="s">
-        <v>131</v>
+        <v>135</v>
       </c>
       <c r="E48" t="s">
-        <v>132</v>
+        <v>136</v>
       </c>
     </row>
     <row r="49" spans="1:7">
       <c r="C49" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="E49" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
     </row>
     <row r="50" spans="1:7">
       <c r="C50" t="s">
-        <v>135</v>
+        <v>139</v>
+      </c>
+      <c r="D50" t="s">
+        <v>140</v>
       </c>
       <c r="E50" t="s">
-        <v>136</v>
+        <v>141</v>
       </c>
     </row>
     <row r="51" spans="1:7">
-      <c r="C51" t="s">
-        <v>137</v>
+      <c r="B51" t="s">
+        <v>142</v>
       </c>
       <c r="D51" t="s">
-        <v>138</v>
+        <v>143</v>
       </c>
       <c r="E51" t="s">
-        <v>139</v>
+        <v>144</v>
       </c>
     </row>
     <row r="52" spans="1:7">
-      <c r="B52" t="s">
-        <v>140</v>
+      <c r="C52" t="s">
+        <v>145</v>
       </c>
       <c r="D52" t="s">
-        <v>141</v>
+        <v>146</v>
       </c>
       <c r="E52" t="s">
-        <v>142</v>
+        <v>147</v>
       </c>
     </row>
     <row r="53" spans="1:7">
       <c r="C53" t="s">
-        <v>143</v>
+        <v>148</v>
       </c>
       <c r="D53" t="s">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="E53" t="s">
-        <v>145</v>
+        <v>150</v>
       </c>
     </row>
     <row r="54" spans="1:7">
       <c r="C54" t="s">
-        <v>146</v>
+        <v>151</v>
+      </c>
+      <c r="D54" t="s">
+        <v>152</v>
       </c>
       <c r="E54" t="s">
-        <v>147</v>
+        <v>153</v>
       </c>
     </row>
     <row r="55" spans="1:7">
       <c r="C55" t="s">
-        <v>148</v>
+        <v>154</v>
+      </c>
+      <c r="D55" t="s">
+        <v>155</v>
       </c>
       <c r="E55" t="s">
-        <v>149</v>
+        <v>156</v>
       </c>
     </row>
     <row r="56" spans="1:7">
       <c r="C56" t="s">
-        <v>150</v>
+        <v>157</v>
+      </c>
+      <c r="D56" t="s">
+        <v>158</v>
       </c>
       <c r="E56" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
     </row>
     <row r="57" spans="1:7">
-      <c r="C57" t="s">
-        <v>152</v>
+      <c r="B57" t="s">
+        <v>160</v>
       </c>
       <c r="D57" t="s">
-        <v>153</v>
+        <v>161</v>
       </c>
       <c r="E57" t="s">
-        <v>154</v>
+        <v>162</v>
       </c>
     </row>
     <row r="58" spans="1:7">
-      <c r="B58" t="s">
-        <v>155</v>
+      <c r="C58" t="s">
+        <v>163</v>
       </c>
       <c r="D58" t="s">
-        <v>156</v>
+        <v>164</v>
       </c>
       <c r="E58" t="s">
-        <v>157</v>
+        <v>165</v>
       </c>
     </row>
     <row r="59" spans="1:7">
-      <c r="C59" t="s">
-        <v>158</v>
-      </c>
-      <c r="D59" t="s">
-        <v>159</v>
+      <c r="A59" t="s">
+        <v>166</v>
       </c>
       <c r="E59" t="s">
-        <v>160</v>
+        <v>167</v>
       </c>
     </row>
     <row r="60" spans="1:7">
       <c r="B60" t="s">
-        <v>161</v>
+        <v>168</v>
+      </c>
+      <c r="D60" t="s">
+        <v>169</v>
       </c>
       <c r="E60" t="s">
-        <v>162</v>
+        <v>170</v>
       </c>
     </row>
     <row r="61" spans="1:7">
-      <c r="C61" t="s">
-        <v>133</v>
+      <c r="B61" t="s">
+        <v>171</v>
+      </c>
+      <c r="D61" t="s">
+        <v>172</v>
       </c>
       <c r="E61" t="s">
-        <v>163</v>
+        <v>173</v>
       </c>
     </row>
     <row r="62" spans="1:7">
       <c r="C62" t="s">
-        <v>135</v>
+        <v>174</v>
+      </c>
+      <c r="D62" t="s">
+        <v>175</v>
       </c>
       <c r="E62" t="s">
-        <v>164</v>
+        <v>176</v>
       </c>
     </row>
     <row r="63" spans="1:7">
-      <c r="A63" t="s">
-        <v>165</v>
+      <c r="C63" t="s">
+        <v>177</v>
+      </c>
+      <c r="D63" t="s">
+        <v>178</v>
       </c>
       <c r="E63" t="s">
-        <v>166</v>
+        <v>179</v>
       </c>
     </row>
     <row r="64" spans="1:7">
-      <c r="B64" t="s">
-        <v>167</v>
+      <c r="C64" t="s">
+        <v>180</v>
       </c>
       <c r="D64" t="s">
-        <v>168</v>
+        <v>181</v>
       </c>
       <c r="E64" t="s">
-        <v>169</v>
+        <v>182</v>
       </c>
     </row>
     <row r="65" spans="1:7">
-      <c r="B65" t="s">
-        <v>170</v>
+      <c r="C65" t="s">
+        <v>183</v>
       </c>
       <c r="D65" t="s">
-        <v>171</v>
+        <v>184</v>
       </c>
       <c r="E65" t="s">
-        <v>172</v>
+        <v>185</v>
       </c>
     </row>
     <row r="66" spans="1:7">
       <c r="C66" t="s">
-        <v>173</v>
+        <v>186</v>
       </c>
       <c r="D66" t="s">
-        <v>174</v>
+        <v>187</v>
       </c>
       <c r="E66" t="s">
-        <v>175</v>
+        <v>188</v>
       </c>
     </row>
     <row r="67" spans="1:7">
       <c r="C67" t="s">
-        <v>176</v>
+        <v>189</v>
       </c>
       <c r="D67" t="s">
-        <v>177</v>
+        <v>190</v>
       </c>
       <c r="E67" t="s">
-        <v>178</v>
+        <v>191</v>
       </c>
     </row>
     <row r="68" spans="1:7">
       <c r="C68" t="s">
-        <v>179</v>
+        <v>192</v>
       </c>
       <c r="D68" t="s">
-        <v>180</v>
+        <v>193</v>
       </c>
       <c r="E68" t="s">
-        <v>181</v>
+        <v>194</v>
       </c>
     </row>
     <row r="69" spans="1:7">
       <c r="C69" t="s">
-        <v>182</v>
+        <v>195</v>
       </c>
       <c r="D69" t="s">
-        <v>183</v>
+        <v>196</v>
       </c>
       <c r="E69" t="s">
-        <v>184</v>
+        <v>197</v>
       </c>
     </row>
     <row r="70" spans="1:7">
       <c r="C70" t="s">
-        <v>185</v>
+        <v>198</v>
       </c>
       <c r="D70" t="s">
-        <v>186</v>
+        <v>199</v>
       </c>
       <c r="E70" t="s">
-        <v>187</v>
+        <v>200</v>
       </c>
     </row>
     <row r="71" spans="1:7">
       <c r="C71" t="s">
-        <v>188</v>
+        <v>201</v>
       </c>
       <c r="D71" t="s">
-        <v>189</v>
+        <v>202</v>
       </c>
       <c r="E71" t="s">
-        <v>190</v>
+        <v>203</v>
       </c>
     </row>
     <row r="72" spans="1:7">
       <c r="C72" t="s">
-        <v>191</v>
+        <v>204</v>
       </c>
       <c r="D72" t="s">
-        <v>192</v>
+        <v>205</v>
       </c>
       <c r="E72" t="s">
-        <v>193</v>
+        <v>206</v>
       </c>
     </row>
     <row r="73" spans="1:7">
-      <c r="C73" t="s">
-        <v>194</v>
+      <c r="B73" t="s">
+        <v>207</v>
       </c>
       <c r="D73" t="s">
-        <v>195</v>
+        <v>208</v>
       </c>
       <c r="E73" t="s">
-        <v>196</v>
+        <v>209</v>
       </c>
     </row>
     <row r="74" spans="1:7">
       <c r="C74" t="s">
-        <v>197</v>
+        <v>210</v>
       </c>
       <c r="D74" t="s">
-        <v>198</v>
+        <v>211</v>
       </c>
       <c r="E74" t="s">
-        <v>199</v>
+        <v>212</v>
       </c>
     </row>
     <row r="75" spans="1:7">
       <c r="C75" t="s">
-        <v>200</v>
-      </c>
-      <c r="D75" t="s">
-        <v>201</v>
+        <v>213</v>
       </c>
       <c r="E75" t="s">
-        <v>202</v>
+        <v>214</v>
       </c>
     </row>
     <row r="76" spans="1:7">
       <c r="C76" t="s">
-        <v>203</v>
-      </c>
-      <c r="D76" t="s">
-        <v>204</v>
+        <v>215</v>
       </c>
       <c r="E76" t="s">
-        <v>205</v>
+        <v>216</v>
       </c>
     </row>
     <row r="77" spans="1:7">
-      <c r="B77" t="s">
-        <v>206</v>
+      <c r="C77" t="s">
+        <v>217</v>
       </c>
       <c r="D77" t="s">
-        <v>207</v>
+        <v>218</v>
       </c>
       <c r="E77" t="s">
-        <v>208</v>
+        <v>219</v>
       </c>
     </row>
     <row r="78" spans="1:7">
       <c r="C78" t="s">
-        <v>209</v>
+        <v>220</v>
       </c>
       <c r="D78" t="s">
-        <v>210</v>
+        <v>221</v>
       </c>
       <c r="E78" t="s">
-        <v>211</v>
+        <v>222</v>
       </c>
     </row>
     <row r="79" spans="1:7">
       <c r="C79" t="s">
-        <v>212</v>
+        <v>223</v>
+      </c>
+      <c r="D79" t="s">
+        <v>224</v>
       </c>
       <c r="E79" t="s">
-        <v>213</v>
+        <v>225</v>
       </c>
     </row>
     <row r="80" spans="1:7">
       <c r="C80" t="s">
-        <v>214</v>
+        <v>226</v>
+      </c>
+      <c r="D80" t="s">
+        <v>227</v>
       </c>
       <c r="E80" t="s">
-        <v>215</v>
+        <v>228</v>
       </c>
     </row>
     <row r="81" spans="1:7">
       <c r="C81" t="s">
-        <v>216</v>
-      </c>
-      <c r="D81" t="s">
-        <v>217</v>
+        <v>229</v>
       </c>
       <c r="E81" t="s">
-        <v>218</v>
+        <v>230</v>
       </c>
     </row>
     <row r="82" spans="1:7">
       <c r="C82" t="s">
-        <v>219</v>
+        <v>231</v>
       </c>
       <c r="D82" t="s">
-        <v>220</v>
+        <v>232</v>
       </c>
       <c r="E82" t="s">
-        <v>221</v>
+        <v>233</v>
       </c>
     </row>
     <row r="83" spans="1:7">
       <c r="C83" t="s">
-        <v>222</v>
+        <v>234</v>
       </c>
       <c r="D83" t="s">
-        <v>223</v>
+        <v>235</v>
       </c>
       <c r="E83" t="s">
-        <v>224</v>
+        <v>236</v>
       </c>
     </row>
     <row r="84" spans="1:7">
       <c r="C84" t="s">
-        <v>225</v>
+        <v>237</v>
       </c>
       <c r="D84" t="s">
-        <v>226</v>
+        <v>238</v>
       </c>
       <c r="E84" t="s">
-        <v>227</v>
+        <v>239</v>
       </c>
     </row>
     <row r="85" spans="1:7">
       <c r="C85" t="s">
-        <v>228</v>
+        <v>240</v>
+      </c>
+      <c r="D85" t="s">
+        <v>241</v>
       </c>
       <c r="E85" t="s">
-        <v>229</v>
+        <v>242</v>
       </c>
     </row>
     <row r="86" spans="1:7">
       <c r="C86" t="s">
-        <v>230</v>
+        <v>243</v>
       </c>
       <c r="D86" t="s">
-        <v>231</v>
+        <v>244</v>
       </c>
       <c r="E86" t="s">
-        <v>232</v>
+        <v>245</v>
       </c>
     </row>
     <row r="87" spans="1:7">
       <c r="C87" t="s">
-        <v>233</v>
+        <v>246</v>
       </c>
       <c r="D87" t="s">
-        <v>234</v>
+        <v>247</v>
       </c>
       <c r="E87" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="88" spans="1:7">
-      <c r="C88" t="s">
-        <v>236</v>
-      </c>
-      <c r="D88" t="s">
-        <v>237</v>
-      </c>
-      <c r="E88" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="89" spans="1:7">
-      <c r="C89" t="s">
-        <v>239</v>
-      </c>
-      <c r="D89" t="s">
-        <v>240</v>
-      </c>
-      <c r="E89" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="90" spans="1:7">
-      <c r="C90" t="s">
-        <v>242</v>
-      </c>
-      <c r="D90" t="s">
-        <v>243</v>
-      </c>
-      <c r="E90" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="91" spans="1:7">
-      <c r="C91" t="s">
-        <v>245</v>
-      </c>
-      <c r="D91" t="s">
-        <v>246</v>
-      </c>
-      <c r="E91" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
     </row>
   </sheetData>

</xml_diff>